<commit_message>
Mise à jour : suivi_web.py, produits.xlsx, requirements.txt et logo
</commit_message>
<xml_diff>
--- a/produits.xlsx
+++ b/produits.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Produits" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,43 +434,53 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Designation</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Dose</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Cible</t>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>dose</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cible</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>mode_d_application</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>vertimec</t>
+          <t>ortiva</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>50 cc/hl</t>
+          <t>50cc/hl</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>acariens</t>
+          <t>oidium</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>feuilles</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ortiva</t>
+          <t>vertimec</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -471,21 +493,9 @@
           <t>oidium</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Test </t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Hiba </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Zwina </t>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>feuilles</t>
         </is>
       </c>
     </row>

</xml_diff>